<commit_message>
Edited to use new Excel file
</commit_message>
<xml_diff>
--- a/public/Rt366.xlsx
+++ b/public/Rt366.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="72">
+  <si>
+    <t xml:space="preserve">New Route</t>
+  </si>
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -247,6 +250,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -416,21 +420,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D53" activeCellId="0" sqref="D53"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.5"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -442,10 +446,13 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>4</v>
+      <c r="A2" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>5</v>
@@ -453,74 +460,92 @@
       <c r="C2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="0" t="n">
+        <v>366</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>9</v>
+      <c r="A4" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>11</v>
+      <c r="A5" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>13</v>
+      <c r="A6" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>14</v>
+      <c r="A7" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>16</v>
+      <c r="A8" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>17</v>
@@ -531,565 +556,706 @@
       <c r="D8" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="E8" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>20</v>
+      <c r="A9" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>5</v>
+        <v>18</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>21</v>
+      <c r="A10" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>22</v>
+      <c r="A11" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>23</v>
+      <c r="A12" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>5</v>
+        <v>25</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>25</v>
+      <c r="A13" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="0" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="0" t="n">
+        <v>366</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>366</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>366</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="0" t="n">
+      <c r="E16" s="0" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>30</v>
+      <c r="A17" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>31</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>5</v>
+        <v>32</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="0" t="n">
+        <v>366</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>5</v>
+      <c r="D18" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>33</v>
+      <c r="A19" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>5</v>
+        <v>32</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>34</v>
+      <c r="A20" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>35</v>
+        <v>19</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="0" t="n">
+        <v>366</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>366</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>366</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>366</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>366</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="0" t="n">
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>366</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="0" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>42</v>
+      <c r="A27" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>43</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>5</v>
+        <v>44</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>44</v>
+      <c r="A28" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>45</v>
+      <c r="A29" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>46</v>
+      <c r="A30" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="0" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>47</v>
+      <c r="A31" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>48</v>
+      <c r="A32" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>49</v>
+      <c r="A33" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>18</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>35</v>
+        <v>19</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>50</v>
+      <c r="A34" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D34" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>51</v>
+      <c r="A35" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>52</v>
+      <c r="A36" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>5</v>
+        <v>25</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>53</v>
+      <c r="A37" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="0" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>54</v>
+      <c r="A38" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>5</v>
+        <v>32</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>55</v>
+      <c r="A39" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D39" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E39" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>56</v>
+      <c r="A40" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>35</v>
+        <v>19</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>57</v>
+      <c r="A41" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>58</v>
+      <c r="A42" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>59</v>
+      <c r="A43" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>60</v>
+      <c r="A44" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>5</v>
+        <v>25</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>61</v>
+      <c r="A45" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>62</v>
+      <c r="A46" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>63</v>
+      <c r="A47" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>64</v>
+      <c r="A48" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>65</v>
+      <c r="A49" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D49" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
-        <v>66</v>
+      <c r="A50" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
-        <v>67</v>
+      <c r="A51" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
-        <v>68</v>
+      <c r="A52" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="E52" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
-        <v>69</v>
+      <c r="A53" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>5</v>
+        <v>32</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
-        <v>70</v>
+      <c r="A54" s="0" t="n">
+        <v>366</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>5</v>
+        <v>25</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Schedule can be viewed daily for the year
</commit_message>
<xml_diff>
--- a/public/Rt366.xlsx
+++ b/public/Rt366.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Call Days</t>
+    <t xml:space="preserve">Days</t>
   </si>
   <si>
     <t xml:space="preserve">Frequency</t>
@@ -422,8 +422,8 @@
   </sheetPr>
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>